<commit_message>
Test all advanced functions
</commit_message>
<xml_diff>
--- a/dat/missing_data.xlsx
+++ b/dat/missing_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="8580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,8 +1158,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <f ca="1">Sheet1!B3+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.2278289386066277</v>
+        <v>7.2278289386066277</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,8 +1166,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">Sheet1!B4+2-RANDBETWEEN(-2, 10)</f>
-        <v>12.400725718491412</v>
+        <v>7.4007257184914117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1176,8 +1174,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <f ca="1">Sheet1!B5+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.5661647906767335</v>
+        <v>11.566164790676734</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1185,8 +1182,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">Sheet1!B6+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.6085801416959509</v>
+        <v>-0.39141985830404913</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,8 +1190,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">Sheet1!B7+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.3313508766455584</v>
+        <v>9.3313508766455584</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,7 +1198,6 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="e">
-        <f ca="1">Sheet1!B8+2-RANDBETWEEN(-2, 10)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1212,8 +1206,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <f ca="1">Sheet1!B9+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.930713174668224</v>
+        <v>2.9307131746682238</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,8 +1214,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <f ca="1">Sheet1!B10+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.0232270620873347</v>
+        <v>7.0232270620873347</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,8 +1222,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <f ca="1">Sheet1!B11+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.8785483409538699</v>
+        <v>5.8785483409538699</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1230,6 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <f ca="1">Sheet1!B12+2-RANDBETWEEN(-2, 10)</f>
         <v>-5</v>
       </c>
     </row>
@@ -1248,8 +1238,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <f ca="1">Sheet1!B13+2-RANDBETWEEN(-2, 10)</f>
-        <v>4.5541406999156102</v>
+        <v>10.55414069991561</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,8 +1246,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <f ca="1">Sheet1!B14+2-RANDBETWEEN(-2, 10)</f>
-        <v>13.051482721126007</v>
+        <v>6.0514827211260069</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1266,8 +1254,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <f ca="1">Sheet1!B15+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.2651015771258898</v>
+        <v>3.2651015771258898</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,8 +1262,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <f ca="1">Sheet1!B16+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.2163129660774281</v>
+        <v>2.2163129660774281</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1284,8 +1270,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <f ca="1">Sheet1!B17+2-RANDBETWEEN(-2, 10)</f>
-        <v>4.4628880119723089</v>
+        <v>5.4628880119723089</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1293,8 +1278,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <f ca="1">Sheet1!B18+2-RANDBETWEEN(-2, 10)</f>
-        <v>2</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,8 +1286,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <f ca="1">Sheet1!B19+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.0442654062304193</v>
+        <v>6.0442654062304193</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1311,8 +1294,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2">
-        <f ca="1">Sheet1!B20+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.8280732521335175</v>
+        <v>10.828073252133517</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,8 +1302,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <f ca="1">Sheet1!B21+2-RANDBETWEEN(-2, 10)</f>
-        <v>0.69826166324459393</v>
+        <v>1.6982616632445939</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1329,8 +1310,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <f ca="1">Sheet1!B22+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.4540455954599611</v>
+        <v>8.4540455954599611</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1338,8 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="2">
-        <f ca="1">Sheet1!B23+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.3381104190867212</v>
+        <v>1.3381104190867212</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1347,7 +1326,6 @@
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <f ca="1">Sheet1!B24+2-RANDBETWEEN(-2, 10)</f>
         <v>-2</v>
       </c>
     </row>
@@ -1356,8 +1334,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2">
-        <f ca="1">Sheet1!B25+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.7084303805975356</v>
+        <v>3.7084303805975356</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1365,8 +1342,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2">
-        <f ca="1">Sheet1!B26+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.7303648432781795</v>
+        <v>6.7303648432781795</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1374,8 +1350,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="2">
-        <f ca="1">Sheet1!B27+2-RANDBETWEEN(-2, 10)</f>
-        <v>4.6139620726506028</v>
+        <v>5.6139620726506028</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1383,7 +1358,6 @@
         <v>28</v>
       </c>
       <c r="B28" s="2">
-        <f ca="1">Sheet1!B28+2-RANDBETWEEN(-2, 10)</f>
         <v>-4</v>
       </c>
     </row>
@@ -1392,7 +1366,6 @@
         <v>29</v>
       </c>
       <c r="B29" s="2">
-        <f ca="1">Sheet1!B29+2-RANDBETWEEN(-2, 10)</f>
         <v>8.5732244099326813</v>
       </c>
     </row>
@@ -1401,8 +1374,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="2">
-        <f ca="1">Sheet1!B30+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.4402984716108147</v>
+        <v>1.4402984716108147</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1410,8 +1382,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="2">
-        <f ca="1">Sheet1!B31+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.3230020326209413</v>
+        <v>-0.67699796737905871</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1419,8 +1390,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="2">
-        <f ca="1">Sheet1!B32+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.5693571814328529</v>
+        <v>13.569357181432853</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,8 +1398,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="2">
-        <f ca="1">Sheet1!B33+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.3823767276049743</v>
+        <v>1.3823767276049743</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1437,8 +1406,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2">
-        <f ca="1">Sheet1!B34+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.0793542013169812</v>
+        <v>7.9354201316981232E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1414,6 @@
         <v>35</v>
       </c>
       <c r="B35" s="2">
-        <f ca="1">Sheet1!B35+2-RANDBETWEEN(-2, 10)</f>
         <v>7.7174989795009541</v>
       </c>
     </row>
@@ -1455,8 +1422,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="2">
-        <f ca="1">Sheet1!B36+2-RANDBETWEEN(-2, 10)</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,8 +1430,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="2">
-        <f ca="1">Sheet1!B37+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.5010843734137751</v>
+        <v>-1.4989156265862249</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1473,8 +1438,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="2">
-        <f ca="1">Sheet1!B38+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.0048071379481929</v>
+        <v>2.0048071379481929</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1482,7 +1446,6 @@
         <v>39</v>
       </c>
       <c r="B39" s="2">
-        <f ca="1">Sheet1!B39+2-RANDBETWEEN(-2, 10)</f>
         <v>7.6263879143713176</v>
       </c>
     </row>
@@ -1491,8 +1454,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="2">
-        <f ca="1">Sheet1!B40+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.7772400638273886</v>
+        <v>7.7772400638273886</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,8 +1462,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="2">
-        <f ca="1">Sheet1!B41+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.146472975659657</v>
+        <v>8.1464729756596572</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1509,8 +1470,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="2">
-        <f ca="1">Sheet1!B42+2-RANDBETWEEN(-2, 10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,8 +1478,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="2">
-        <f ca="1">Sheet1!B43+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.115788574260812</v>
+        <v>13.115788574260812</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,8 +1486,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="2">
-        <f ca="1">Sheet1!B44+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.7888154326051797</v>
+        <v>1.7888154326051797</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,8 +1494,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="2">
-        <f ca="1">Sheet1!B45+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.2073463415950823</v>
+        <v>7.2073463415950823</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1545,8 +1502,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="2">
-        <f ca="1">Sheet1!B46+2-RANDBETWEEN(-2, 10)</f>
-        <v>0.5272840558665699</v>
+        <v>2.5272840558665699</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1554,8 +1510,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="2">
-        <f ca="1">Sheet1!B47+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.2243284437983455</v>
+        <v>2.2243284437983455</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,8 +1518,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="2">
-        <f ca="1">Sheet1!B48+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.1519358798135</v>
+        <v>6.1519358798135002</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1572,8 +1526,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="2">
-        <f ca="1">Sheet1!B49+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.7569116956588857</v>
+        <v>3.7569116956588857</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1581,8 +1534,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="2">
-        <f ca="1">Sheet1!B50+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.9880620654125565</v>
+        <v>4.9880620654125565</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1590,8 +1542,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="2">
-        <f ca="1">Sheet1!B51+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.7490751506767142</v>
+        <v>-0.25092484932328585</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1599,8 +1550,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="2">
-        <f ca="1">Sheet1!B52+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.2986600136733113</v>
+        <v>13.298660013673311</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,8 +1558,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="2">
-        <f ca="1">Sheet1!B53+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.7435519737218925</v>
+        <v>12.743551973721893</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,8 +1566,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="2">
-        <f ca="1">Sheet1!B54+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.5771592996044905</v>
+        <v>3.5771592996044905</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1626,8 +1574,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="2">
-        <f ca="1">Sheet1!B55+2-RANDBETWEEN(-2, 10)</f>
-        <v>-1.2719571878122711</v>
+        <v>5.7280428121877289</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,8 +1582,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="2">
-        <f ca="1">Sheet1!B56+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.8969919821561341</v>
+        <v>4.8969919821561341</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1644,8 +1590,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="2">
-        <f ca="1">Sheet1!B57+2-RANDBETWEEN(-2, 10)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,8 +1598,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="2">
-        <f ca="1">Sheet1!B58+2-RANDBETWEEN(-2, 10)</f>
-        <v>12.988182468252074</v>
+        <v>4.9881824682520737</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1662,8 +1606,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="2">
-        <f ca="1">Sheet1!B59+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.581297436311575</v>
+        <v>9.5812974363115746</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1671,8 +1614,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="2">
-        <f ca="1">Sheet1!B60+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.3484810683254747</v>
+        <v>8.3484810683254747</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,8 +1622,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="2">
-        <f ca="1">Sheet1!B61+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.9478560158421843</v>
+        <v>11.947856015842184</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1689,8 +1630,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="2">
-        <f ca="1">Sheet1!B62+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.458732083009588</v>
+        <v>8.458732083009588</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,8 +1638,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="2">
-        <f ca="1">Sheet1!B63+2-RANDBETWEEN(-2, 10)</f>
-        <v>-0.99292399714633994</v>
+        <v>1.0070760028536601</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1707,8 +1646,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="2">
-        <f ca="1">Sheet1!B64+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.5203906801741596</v>
+        <v>10.52039068017416</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,8 +1654,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="2">
-        <f ca="1">Sheet1!B65+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.0383891633866469</v>
+        <v>4.0383891633866469</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,8 +1662,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="2">
-        <f ca="1">Sheet1!B66+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.4603693360951642</v>
+        <v>11.460369336095164</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1746,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1704,6 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <f>3</f>
         <v>3</v>
       </c>
     </row>
@@ -1777,8 +1712,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <f ca="1">Sheet1!B3+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.2278289386066277</v>
+        <v>2.2278289386066277</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1786,8 +1720,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">Sheet1!B4+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.4007257184914117</v>
+        <v>7.4007257184914117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1795,8 +1728,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <f ca="1">Sheet1!B5+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.5661647906767335</v>
+        <v>4.5661647906767335</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1804,8 +1736,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">Sheet1!B6+2-RANDBETWEEN(-2, 10)</f>
-        <v>-0.39141985830404913</v>
+        <v>-2.3914198583040491</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1813,8 +1744,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">Sheet1!B7+2-RANDBETWEEN(-2, 10)</f>
-        <v>12.331350876645558</v>
+        <v>10.331350876645558</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1822,7 +1752,6 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="e">
-        <f ca="1">Sheet1!B8+2-RANDBETWEEN(-2, 10)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1831,8 +1760,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <f ca="1">Sheet1!B9+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.9307131746682238</v>
+        <v>4.9307131746682238</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,8 +1768,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <f ca="1">Sheet1!B10+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.0232270620873347</v>
+        <v>7.0232270620873347</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1849,8 +1776,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <f ca="1">Sheet1!B11+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.8785483409538699</v>
+        <v>10.87854834095387</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1858,8 +1784,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <f ca="1">Sheet1!B12+2-RANDBETWEEN(-2, 10)</f>
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1867,8 +1792,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <f ca="1">Sheet1!B13+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.55414069991561</v>
+        <v>3.5541406999156102</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1876,8 +1800,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <f ca="1">Sheet1!B14+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.0514827211260069</v>
+        <v>10.051482721126007</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1885,8 +1808,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <f ca="1">Sheet1!B15+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.2651015771258898</v>
+        <v>2.2651015771258898</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,8 +1816,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <f ca="1">Sheet1!B16+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.2163129660774281</v>
+        <v>9.2163129660774281</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1903,8 +1824,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <f ca="1">Sheet1!B17+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.4628880119723089</v>
+        <v>-0.53711198802769111</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,8 +1832,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <f ca="1">Sheet1!B18+2-RANDBETWEEN(-2, 10)</f>
-        <v>-8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,8 +1840,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <f ca="1">Sheet1!B19+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.0442654062304193</v>
+        <v>4.0442654062304193</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,8 +1848,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2">
-        <f ca="1">Sheet1!B20+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.828073252133517</v>
+        <v>5.8280732521335175</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1939,8 +1856,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <f ca="1">Sheet1!B21+2-RANDBETWEEN(-2, 10)</f>
-        <v>7.6982616632445939</v>
+        <v>8.6982616632445939</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1948,8 +1864,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <f ca="1">Sheet1!B22+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.4540455954599611</v>
+        <v>2.4540455954599611</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,7 +1872,6 @@
         <v>23</v>
       </c>
       <c r="B23" s="2">
-        <f ca="1">Sheet1!B23+2-RANDBETWEEN(-2, 10)</f>
         <v>13.338110419086721</v>
       </c>
     </row>
@@ -1966,8 +1880,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <f ca="1">Sheet1!B24+2-RANDBETWEEN(-2, 10)</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1975,8 +1888,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2">
-        <f ca="1">Sheet1!B25+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.708430380597536</v>
+        <v>8.7084303805975356</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,8 +1896,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2">
-        <f ca="1">Sheet1!B26+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.7303648432781795</v>
+        <v>4.7303648432781795</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1993,8 +1904,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="2">
-        <f ca="1">Sheet1!B27+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.6139620726506028</v>
+        <v>4.6139620726506028</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2002,8 +1912,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="2">
-        <f ca="1">Sheet1!B28+2-RANDBETWEEN(-2, 10)</f>
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2011,7 +1920,6 @@
         <v>29</v>
       </c>
       <c r="B29" s="2">
-        <f ca="1">Sheet1!B29+2-RANDBETWEEN(-2, 10)</f>
         <v>4.5732244099326813</v>
       </c>
     </row>
@@ -2020,8 +1928,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="2">
-        <f ca="1">Sheet1!B30+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.4402984716108147</v>
+        <v>10.440298471610815</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2029,8 +1936,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="2">
-        <f ca="1">Sheet1!B31+2-RANDBETWEEN(-2, 10)</f>
-        <v>-0.67699796737905871</v>
+        <v>-1.6769979673790587</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,8 +1944,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="2">
-        <f ca="1">Sheet1!B32+2-RANDBETWEEN(-2, 10)</f>
-        <v>13.569357181432853</v>
+        <v>5.5693571814328529</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,8 +1952,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="2">
-        <f ca="1">Sheet1!B33+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.3823767276049743</v>
+        <v>10.382376727604974</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2056,8 +1960,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2">
-        <f ca="1">Sheet1!B34+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.0793542013169812</v>
+        <v>5.0793542013169812</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2065,7 +1968,6 @@
         <v>35</v>
       </c>
       <c r="B35" s="2">
-        <f ca="1">Sheet1!B35+2-RANDBETWEEN(-2, 10)</f>
         <v>13.717498979500954</v>
       </c>
     </row>
@@ -2074,8 +1976,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="2">
-        <f ca="1">Sheet1!B36+2-RANDBETWEEN(-2, 10)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,8 +1984,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="2">
-        <f ca="1">Sheet1!B37+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.5010843734137751</v>
+        <v>4.5010843734137751</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2092,8 +1992,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="2">
-        <f ca="1">Sheet1!B38+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.0048071379481929</v>
+        <v>7.0048071379481929</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,8 +2000,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="2">
-        <f ca="1">Sheet1!B39+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.6263879143713176</v>
+        <v>0.62638791437131758</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,8 +2008,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="2">
-        <f ca="1">Sheet1!B40+2-RANDBETWEEN(-2, 10)</f>
-        <v>8.7772400638273886</v>
+        <v>1.7772400638273886</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2119,7 +2016,6 @@
         <v>41</v>
       </c>
       <c r="B41" s="2">
-        <f ca="1">Sheet1!B41+2-RANDBETWEEN(-2, 10)</f>
         <v>11.146472975659657</v>
       </c>
     </row>
@@ -2128,8 +2024,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="2">
-        <f ca="1">Sheet1!B42+2-RANDBETWEEN(-2, 10)</f>
-        <v>-7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,8 +2032,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="2">
-        <f ca="1">Sheet1!B43+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.115788574260812</v>
+        <v>5.1157885742608116</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2146,8 +2040,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="2">
-        <f ca="1">Sheet1!B44+2-RANDBETWEEN(-2, 10)</f>
-        <v>-1.2111845673948203</v>
+        <v>1.7888154326051797</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,8 +2048,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="2">
-        <f ca="1">Sheet1!B45+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.2073463415950823</v>
+        <v>7.2073463415950823</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2164,8 +2056,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="2">
-        <f ca="1">Sheet1!B46+2-RANDBETWEEN(-2, 10)</f>
-        <v>-1.4727159441334301</v>
+        <v>-0.4727159441334301</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,8 +2064,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="2">
-        <f ca="1">Sheet1!B47+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.2243284437983455</v>
+        <v>6.2243284437983455</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2182,8 +2072,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="2">
-        <f ca="1">Sheet1!B48+2-RANDBETWEEN(-2, 10)</f>
-        <v>6.1519358798135002</v>
+        <v>2.1519358798135002</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2191,8 +2080,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="2">
-        <f ca="1">Sheet1!B49+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.7569116956588857</v>
+        <v>0.75691169565888572</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,8 +2088,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="2">
-        <f ca="1">Sheet1!B50+2-RANDBETWEEN(-2, 10)</f>
-        <v>13.988062065412556</v>
+        <v>2.9880620654125565</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2096,6 @@
         <v>51</v>
       </c>
       <c r="B51" s="2">
-        <f ca="1">Sheet1!B51+2-RANDBETWEEN(-2, 10)</f>
         <v>9.7490751506767133</v>
       </c>
     </row>
@@ -2218,8 +2104,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="2">
-        <f ca="1">Sheet1!B52+2-RANDBETWEEN(-2, 10)</f>
-        <v>10.298660013673311</v>
+        <v>8.2986600136733113</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,8 +2112,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="2">
-        <f ca="1">Sheet1!B53+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.7435519737218925</v>
+        <v>6.7435519737218925</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2236,8 +2120,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="2">
-        <f ca="1">Sheet1!B54+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.5771592996044905</v>
+        <v>13.577159299604491</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,8 +2128,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="2">
-        <f ca="1">Sheet1!B55+2-RANDBETWEEN(-2, 10)</f>
-        <v>2.7280428121877289</v>
+        <v>3.7280428121877289</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2254,8 +2136,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="2">
-        <f ca="1">Sheet1!B56+2-RANDBETWEEN(-2, 10)</f>
-        <v>9.8969919821561341</v>
+        <v>3.8969919821561341</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,8 +2144,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="2">
-        <f ca="1">Sheet1!B57+2-RANDBETWEEN(-2, 10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,8 +2152,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="2">
-        <f ca="1">Sheet1!B58+2-RANDBETWEEN(-2, 10)</f>
-        <v>5.9881824682520737</v>
+        <v>9.9881824682520737</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2160,6 @@
         <v>59</v>
       </c>
       <c r="B59" s="2">
-        <f ca="1">Sheet1!B59+2-RANDBETWEEN(-2, 10)</f>
         <v>-0.4187025636884254</v>
       </c>
     </row>
@@ -2290,8 +2168,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="2">
-        <f ca="1">Sheet1!B60+2-RANDBETWEEN(-2, 10)</f>
-        <v>11.348481068325475</v>
+        <v>2.3484810683254747</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2299,8 +2176,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="2">
-        <f ca="1">Sheet1!B61+2-RANDBETWEEN(-2, 10)</f>
-        <v>4.9478560158421843</v>
+        <v>12.947856015842184</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2308,7 +2184,6 @@
         <v>62</v>
       </c>
       <c r="B62" s="2">
-        <f ca="1">Sheet1!B62+2-RANDBETWEEN(-2, 10)</f>
         <v>7.458732083009588</v>
       </c>
     </row>
@@ -2317,8 +2192,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="2">
-        <f ca="1">Sheet1!B63+2-RANDBETWEEN(-2, 10)</f>
-        <v>1.0070760028536601</v>
+        <v>11.00707600285366</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2326,8 +2200,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="2">
-        <f ca="1">Sheet1!B64+2-RANDBETWEEN(-2, 10)</f>
-        <v>3.5203906801741596</v>
+        <v>6.5203906801741596</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2335,8 +2208,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="2">
-        <f ca="1">Sheet1!B65+2-RANDBETWEEN(-2, 10)</f>
-        <v>4.0383891633866469</v>
+        <v>3.8389163386646885E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2344,7 +2216,6 @@
         <v>66</v>
       </c>
       <c r="B66" s="2">
-        <f ca="1">Sheet1!B66+2-RANDBETWEEN(-2, 10)</f>
         <v>13.460369336095164</v>
       </c>
     </row>

</xml_diff>